<commit_message>
Created planet class. Testing planet class acceleration method. Writing report.
	modified:   Reports/Project Report.docx
	new file:   Reports/Success Criteria.docx
	modified:   Reports/Test Data Book.xlsx
	modified:   Reports/~$oject Report.docx
	new file:   __pycache__/planet_class.cpython-310.pyc
	modified:   __pycache__/vector_class.cpython-310.pyc
	new file:   planet_class.py
	modified:   testing.py
	modified:   vector_class.py
</commit_message>
<xml_diff>
--- a/Reports/Test Data Book.xlsx
+++ b/Reports/Test Data Book.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Desktop\school\Computer Science\Project\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591C00AC-5E2B-4D60-BD1D-1A47F4817CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F75202-92A9-4E6E-BC46-68344ACB87ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{529305D3-BB45-46FD-90A7-933F6ADD743A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>planet index</t>
   </si>
@@ -90,6 +90,21 @@
   </si>
   <si>
     <t>y (B--&gt;A) unit vec (m)</t>
+  </si>
+  <si>
+    <t>Planet</t>
+  </si>
+  <si>
+    <t>Resultant x</t>
+  </si>
+  <si>
+    <t>Resultant y</t>
+  </si>
+  <si>
+    <t>Acceleration x</t>
+  </si>
+  <si>
+    <t>Acceleration y</t>
   </si>
 </sst>
 </file>
@@ -481,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD25F577-0A0D-4096-BEC1-930925B3B023}">
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:Y21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X5" sqref="X5:Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -506,9 +521,13 @@
     <col min="18" max="18" width="15.77734375" customWidth="1"/>
     <col min="19" max="19" width="17" customWidth="1"/>
     <col min="20" max="20" width="20.21875" customWidth="1"/>
+    <col min="21" max="21" width="12.88671875" customWidth="1"/>
+    <col min="22" max="23" width="15" customWidth="1"/>
+    <col min="24" max="24" width="17" customWidth="1"/>
+    <col min="25" max="25" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -563,8 +582,23 @@
       <c r="S1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -632,8 +666,27 @@
         <f>6.6743 * 10 ^ -11</f>
         <v>6.6742999999999994E-11</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <f>SUM(N2, N3, N4, N5)</f>
+        <v>1.8957062822219974E+21</v>
+      </c>
+      <c r="W2">
+        <f>SUM(O2, O3, O4, O5)</f>
+        <v>3.0360319521610515E+21</v>
+      </c>
+      <c r="X2">
+        <f>V2/B2</f>
+        <v>6.217468947923902E-4</v>
+      </c>
+      <c r="Y2">
+        <f>W2/B2</f>
+        <v>9.9574678654019413E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -697,8 +750,27 @@
         <f t="shared" ref="Q3:Q21" si="1" xml:space="preserve"> -O3</f>
         <v>-1.3799639756067102E+17</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U3">
+        <v>2</v>
+      </c>
+      <c r="V3">
+        <f>SUM(N6,N7,N8,P2)</f>
+        <v>-9.0841269225517975E+21</v>
+      </c>
+      <c r="W3">
+        <f>SUM(O8,O7,O6,Q2)</f>
+        <v>7.8191254034914424E+21</v>
+      </c>
+      <c r="X3">
+        <f t="shared" ref="X3:X6" si="2">V3/B3</f>
+        <v>-1.4819130379366717E-3</v>
+      </c>
+      <c r="Y3">
+        <f t="shared" ref="Y3:Y6" si="3">W3/B3</f>
+        <v>1.2755506367849009E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -707,11 +779,11 @@
         <v>2.2899999999999998E+23</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ref="C4" si="2">E4*1.496 * 10 ^ 8</f>
+        <f t="shared" ref="C4" si="4">E4*1.496 * 10 ^ 8</f>
         <v>9080720000</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:D14" si="3">F4*1.496*10^8</f>
+        <f t="shared" ref="D4:D14" si="5">F4*1.496*10^8</f>
         <v>15334000000</v>
       </c>
       <c r="E4" s="1">
@@ -739,11 +811,11 @@
         <v>0.94705883866766827</v>
       </c>
       <c r="L4" s="4">
-        <f t="shared" ref="L4:L21" si="4">-J4</f>
+        <f t="shared" ref="L4:L21" si="6">-J4</f>
         <v>-0.32106005061584247</v>
       </c>
       <c r="M4" s="4">
-        <f t="shared" ref="M4:M21" si="5">-K4</f>
+        <f t="shared" ref="M4:M21" si="7">-K4</f>
         <v>-0.94705883866766827</v>
       </c>
       <c r="N4">
@@ -762,8 +834,27 @@
         <f t="shared" si="1"/>
         <v>-2.3740738970755421E+21</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U4">
+        <v>3</v>
+      </c>
+      <c r="V4">
+        <f>SUM(N9,N10,P3,P6)</f>
+        <v>-6.7138465553336333E+17</v>
+      </c>
+      <c r="W4">
+        <f>SUM(O9,O10,Q3,Q6)</f>
+        <v>-1.2987414927331274E+18</v>
+      </c>
+      <c r="X4">
+        <f t="shared" si="2"/>
+        <v>-2.9318107228531152E-6</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" si="3"/>
+        <v>-5.6713602302756664E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -772,11 +863,11 @@
         <v>1.477E+25</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" ref="C5" si="6">E5*1.496*10^8</f>
+        <f t="shared" ref="C5" si="8">E5*1.496*10^8</f>
         <v>568480000</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1900219200</v>
       </c>
       <c r="E5" s="1">
@@ -804,11 +895,11 @@
         <v>0.35416218470606303</v>
       </c>
       <c r="L5" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-0.9351840176800652</v>
       </c>
       <c r="M5" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-0.35416218470606303</v>
       </c>
       <c r="N5">
@@ -827,8 +918,27 @@
         <f xml:space="preserve"> -O5</f>
         <v>-2.3865958018989571E+17</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U5">
+        <v>4</v>
+      </c>
+      <c r="V5">
+        <f>SUM(N11,P4,P7,P9)</f>
+        <v>7.1946104103851168E+21</v>
+      </c>
+      <c r="W5">
+        <f>SUM(O11,Q9,Q7,Q4)</f>
+        <v>-1.0852110566190496E+22</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="2"/>
+        <v>4.8710970957245201E-4</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="3"/>
+        <v>-7.3474005187477965E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -837,11 +947,11 @@
         <v>9.0143999999999992E+23</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" ref="C6" si="7">E6*1.496 * 10 ^ 8</f>
+        <f t="shared" ref="C6" si="9">E6*1.496 * 10 ^ 8</f>
         <v>15646664000.000002</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6706568000</v>
       </c>
       <c r="E6" s="1">
@@ -869,11 +979,11 @@
         <v>0.86710503001820083</v>
       </c>
       <c r="L6" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-0.49812535261431434</v>
       </c>
       <c r="M6" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-0.86710503001820083</v>
       </c>
       <c r="N6">
@@ -892,14 +1002,33 @@
         <f t="shared" si="1"/>
         <v>-3.1353810025395923E+17</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="U6">
+        <v>5</v>
+      </c>
+      <c r="V6">
+        <f>SUM(P11,P10,P8,P5)</f>
+        <v>-5.5183853997845422E+18</v>
+      </c>
+      <c r="W6">
+        <f>SUM(Q11,Q10,Q8,Q5)</f>
+        <v>-1.7480479692639642E+18</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="2"/>
+        <v>-6.1217445418270132E-6</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="3"/>
+        <v>-1.9391728448526405E-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="C7" s="1">
-        <f t="shared" ref="C7" si="8">E7*1.496*10^8</f>
+        <f t="shared" ref="C7" si="10">E7*1.496*10^8</f>
         <v>0</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G7">
@@ -921,11 +1050,11 @@
         <v>0.72757755456562689</v>
       </c>
       <c r="L7" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.68602543837113084</v>
       </c>
       <c r="M7" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-0.72757755456562689</v>
       </c>
       <c r="N7">
@@ -945,13 +1074,13 @@
         <v>-8.4798681837988982E+21</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="C8" s="1">
-        <f t="shared" ref="C8" si="9">E8*1.496 * 10 ^ 8</f>
+        <f t="shared" ref="C8" si="11">E8*1.496 * 10 ^ 8</f>
         <v>0</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G8">
@@ -973,11 +1102,11 @@
         <v>0.3432727173807677</v>
       </c>
       <c r="L8" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-0.93923577524603674</v>
       </c>
       <c r="M8" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-0.3432727173807677</v>
       </c>
       <c r="N8">
@@ -997,13 +1126,13 @@
         <v>-5.2508070004820998E+17</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="C9" s="1">
-        <f t="shared" ref="C9" si="10">E9*1.496*10^8</f>
+        <f t="shared" ref="C9" si="12">E9*1.496*10^8</f>
         <v>0</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G9">
@@ -1025,11 +1154,11 @@
         <v>-0.84470028152533305</v>
       </c>
       <c r="L9" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.53523960465479692</v>
       </c>
       <c r="M9" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.84470028152533305</v>
       </c>
       <c r="N9">
@@ -1049,13 +1178,13 @@
         <v>7.539336073850231E+17</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="C10" s="1">
-        <f t="shared" ref="C10" si="11">E10*1.496 * 10 ^ 8</f>
+        <f t="shared" ref="C10" si="13">E10*1.496 * 10 ^ 8</f>
         <v>0</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G10">
@@ -1077,11 +1206,11 @@
         <v>-0.79575785844926916</v>
       </c>
       <c r="L10" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-0.60561491949607138</v>
       </c>
       <c r="M10" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0.79575785844926916</v>
       </c>
       <c r="N10">
@@ -1101,13 +1230,13 @@
         <v>9.3273387533474032E+16</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="C11" s="1">
-        <f t="shared" ref="C11" si="12">E11*1.496*10^8</f>
+        <f t="shared" ref="C11" si="14">E11*1.496*10^8</f>
         <v>0</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G11">
@@ -1129,11 +1258,11 @@
         <v>0.30370538587989993</v>
       </c>
       <c r="L11" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-0.95276599361414083</v>
       </c>
       <c r="M11" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-0.30370538587989993</v>
       </c>
       <c r="N11">
@@ -1153,73 +1282,73 @@
         <v>-1.0775810765593325E+18</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="C12" s="1">
-        <f t="shared" ref="C12" si="13">E12*1.496 * 10 ^ 8</f>
+        <f t="shared" ref="C12" si="15">E12*1.496 * 10 ^ 8</f>
         <v>0</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L12" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M12" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P12" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="C13" s="1">
+        <f t="shared" ref="C13" si="16">E13*1.496*10^8</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P12" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="C13" s="1">
-        <f t="shared" ref="C13" si="14">E13*1.496*10^8</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="L13" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M13" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="C14" s="1">
+        <f t="shared" ref="C14" si="17">E14*1.496 * 10 ^ 8</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P13" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="C14" s="1">
-        <f t="shared" ref="C14" si="15">E14*1.496 * 10 ^ 8</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
       <c r="L14" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M14" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P14" s="4">
@@ -1231,13 +1360,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="L15" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M15" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P15" s="4">
@@ -1249,13 +1378,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="L16" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M16" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P16" s="4">
@@ -1269,11 +1398,11 @@
     </row>
     <row r="17" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L17" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M17" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P17" s="4">
@@ -1287,11 +1416,11 @@
     </row>
     <row r="18" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L18" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M18" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P18" s="4">
@@ -1305,11 +1434,11 @@
     </row>
     <row r="19" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L19" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M19" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P19" s="4">
@@ -1323,11 +1452,11 @@
     </row>
     <row r="20" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L20" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M20" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P20" s="4">
@@ -1341,11 +1470,11 @@
     </row>
     <row r="21" spans="12:17" x14ac:dyDescent="0.3">
       <c r="L21" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M21" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P21" s="4">
@@ -1359,5 +1488,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new file:   GUI.py 	modified:   Reports/Project Report.docx 	modified:   Reports/References.docx 	modified:   Reports/Success Criteria.docx 	modified:   Reports/Test Data Book.xlsx 	modified:   Reports/~$oject Report.docx 	modified:   __pycache__/planet_class.cpython-310.pyc 	modified:   planet_class.py 	modified:   testing.py
</commit_message>
<xml_diff>
--- a/Reports/Test Data Book.xlsx
+++ b/Reports/Test Data Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Desktop\school\Computer Science\Project\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F75202-92A9-4E6E-BC46-68344ACB87ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B4C4DE-3989-4E5F-AF46-C1E742244814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{529305D3-BB45-46FD-90A7-933F6ADD743A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>planet index</t>
   </si>
@@ -105,6 +105,24 @@
   </si>
   <si>
     <t>Acceleration y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Half V (x) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Half V (y) </t>
+  </si>
+  <si>
+    <t>time step size (s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planet </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos x </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos y </t>
   </si>
 </sst>
 </file>
@@ -120,7 +138,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,6 +157,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -152,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -162,6 +192,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD25F577-0A0D-4096-BEC1-930925B3B023}">
-  <dimension ref="A1:Y21"/>
+  <dimension ref="A1:AA22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5:Y5"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X22" sqref="X22:Y22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,26 +540,26 @@
     <col min="2" max="2" width="13.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="15.6640625" style="1" customWidth="1"/>
-    <col min="7" max="9" width="27.5546875" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" customWidth="1"/>
-    <col min="11" max="11" width="22.5546875" customWidth="1"/>
-    <col min="12" max="12" width="24.5546875" style="4" customWidth="1"/>
-    <col min="13" max="13" width="25.109375" style="4" customWidth="1"/>
-    <col min="14" max="14" width="22" customWidth="1"/>
-    <col min="15" max="15" width="20.21875" customWidth="1"/>
-    <col min="16" max="16" width="20.6640625" style="4" customWidth="1"/>
-    <col min="17" max="17" width="16.109375" style="4" customWidth="1"/>
-    <col min="18" max="18" width="15.77734375" customWidth="1"/>
-    <col min="19" max="19" width="17" customWidth="1"/>
-    <col min="20" max="20" width="20.21875" customWidth="1"/>
-    <col min="21" max="21" width="12.88671875" customWidth="1"/>
-    <col min="22" max="23" width="15" customWidth="1"/>
-    <col min="24" max="24" width="17" customWidth="1"/>
-    <col min="25" max="25" width="14.44140625" customWidth="1"/>
+    <col min="5" max="8" width="15.6640625" style="1" customWidth="1"/>
+    <col min="9" max="11" width="27.5546875" customWidth="1"/>
+    <col min="12" max="12" width="19.6640625" customWidth="1"/>
+    <col min="13" max="13" width="22.5546875" customWidth="1"/>
+    <col min="14" max="14" width="24.5546875" style="4" customWidth="1"/>
+    <col min="15" max="15" width="25.109375" style="4" customWidth="1"/>
+    <col min="16" max="16" width="22" customWidth="1"/>
+    <col min="17" max="17" width="20.21875" customWidth="1"/>
+    <col min="18" max="18" width="20.6640625" style="4" customWidth="1"/>
+    <col min="19" max="19" width="16.109375" style="4" customWidth="1"/>
+    <col min="20" max="20" width="15.77734375" customWidth="1"/>
+    <col min="21" max="21" width="17" customWidth="1"/>
+    <col min="22" max="22" width="20.21875" customWidth="1"/>
+    <col min="23" max="23" width="12.88671875" customWidth="1"/>
+    <col min="24" max="25" width="15" customWidth="1"/>
+    <col min="26" max="26" width="17" customWidth="1"/>
+    <col min="27" max="27" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -546,59 +578,59 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -620,73 +652,73 @@
       <c r="F2" s="1">
         <v>5.77</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>1</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>2</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <f>SQRT((C2-C3)^2 + (D2-D3)^2)</f>
         <v>989058584.27124536</v>
       </c>
-      <c r="J2">
-        <f>(C3-C2)/I2</f>
+      <c r="L2">
+        <f>(C3-C2)/K2</f>
         <v>0.85489293904971986</v>
       </c>
-      <c r="K2">
-        <f>(D3-D2)/I2</f>
+      <c r="M2">
+        <f>(D3-D2)/K2</f>
         <v>0.51880445522656404</v>
       </c>
-      <c r="L2" s="4">
-        <f>-J2</f>
+      <c r="N2" s="4">
+        <f>-L2</f>
         <v>-0.85489293904971986</v>
       </c>
-      <c r="M2" s="4">
-        <f>-K2</f>
+      <c r="O2" s="4">
+        <f>-M2</f>
         <v>-0.51880445522656404</v>
       </c>
-      <c r="N2">
-        <f xml:space="preserve"> -S$2 *(B2 *B3) / (I2)^2 *L2</f>
+      <c r="P2">
+        <f xml:space="preserve"> -U$2 *(B2 *B3) / (K2)^2 *N2</f>
         <v>1.0901627019699858E+21</v>
       </c>
-      <c r="O2">
-        <f xml:space="preserve"> -S$2 *(B2*B3) /(I2 )^2 * M2</f>
+      <c r="Q2">
+        <f xml:space="preserve"> -U$2 *(B2*B3) /(K2 )^2 * O2</f>
         <v>6.6158139910775872E+20</v>
       </c>
-      <c r="P2" s="4">
-        <f xml:space="preserve"> -N2</f>
+      <c r="R2" s="4">
+        <f xml:space="preserve"> -P2</f>
         <v>-1.0901627019699858E+21</v>
       </c>
-      <c r="Q2" s="4">
-        <f xml:space="preserve"> -O2</f>
+      <c r="S2" s="4">
+        <f xml:space="preserve"> -Q2</f>
         <v>-6.6158139910775872E+20</v>
       </c>
-      <c r="S2">
+      <c r="U2">
         <f>6.6743 * 10 ^ -11</f>
         <v>6.6742999999999994E-11</v>
       </c>
-      <c r="U2">
+      <c r="W2" s="1">
         <v>1</v>
       </c>
-      <c r="V2">
-        <f>SUM(N2, N3, N4, N5)</f>
+      <c r="X2" s="1">
+        <f>SUM(P2, P3, P4, P5)</f>
         <v>1.8957062822219974E+21</v>
       </c>
-      <c r="W2">
-        <f>SUM(O2, O3, O4, O5)</f>
+      <c r="Y2" s="1">
+        <f>SUM(Q2, Q3, Q4, Q5)</f>
         <v>3.0360319521610515E+21</v>
       </c>
-      <c r="X2">
-        <f>V2/B2</f>
+      <c r="Z2" s="1">
+        <f>X2/B2</f>
         <v>6.217468947923902E-4</v>
       </c>
-      <c r="Y2">
-        <f>W2/B2</f>
+      <c r="AA2" s="1">
+        <f>Y2/B2</f>
         <v>9.9574678654019413E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -708,69 +740,69 @@
       <c r="F3" s="1">
         <v>9.1999999999999993</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>1</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>3</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <f>SQRT((C2-C4)^2 + (D2-D4)^2)</f>
         <v>16969715218.967701</v>
       </c>
-      <c r="J3">
-        <f>(C4-C2)/I3</f>
+      <c r="L3">
+        <f>(C4-C2)/K3</f>
         <v>0.52233050971253725</v>
       </c>
-      <c r="K3">
-        <f>(D4-D2)/I3</f>
+      <c r="M3">
+        <f>(D4-D2)/K3</f>
         <v>0.85274312581424017</v>
       </c>
-      <c r="L3" s="4">
-        <f>-J3</f>
+      <c r="N3" s="4">
+        <f>-L3</f>
         <v>-0.52233050971253725</v>
       </c>
-      <c r="M3" s="4">
-        <f>-K3</f>
+      <c r="O3" s="4">
+        <f>-M3</f>
         <v>-0.85274312581424017</v>
       </c>
-      <c r="N3">
-        <f xml:space="preserve"> -S$2 *(B2 *B4) / (I3)^2 *L3</f>
+      <c r="P3">
+        <f xml:space="preserve"> -U$2 *(B2 *B4) / (K3)^2 *N3</f>
         <v>8.4526895021914176E+16</v>
       </c>
-      <c r="O3">
-        <f xml:space="preserve"> -S$2 *(B2 *B4) / (I3)^2 *M3</f>
+      <c r="Q3">
+        <f xml:space="preserve"> -U$2 *(B2 *B4) / (K3)^2 *O3</f>
         <v>1.3799639756067102E+17</v>
       </c>
-      <c r="P3" s="4">
-        <f t="shared" ref="P3:P21" si="0" xml:space="preserve"> -N3</f>
+      <c r="R3" s="4">
+        <f t="shared" ref="R3:R21" si="0" xml:space="preserve"> -P3</f>
         <v>-8.4526895021914176E+16</v>
       </c>
-      <c r="Q3" s="4">
-        <f t="shared" ref="Q3:Q21" si="1" xml:space="preserve"> -O3</f>
+      <c r="S3" s="4">
+        <f t="shared" ref="S3:S21" si="1" xml:space="preserve"> -Q3</f>
         <v>-1.3799639756067102E+17</v>
       </c>
-      <c r="U3">
+      <c r="W3" s="1">
         <v>2</v>
       </c>
-      <c r="V3">
-        <f>SUM(N6,N7,N8,P2)</f>
+      <c r="X3" s="1">
+        <f>SUM(P6,P7,P8,R2)</f>
         <v>-9.0841269225517975E+21</v>
       </c>
-      <c r="W3">
-        <f>SUM(O8,O7,O6,Q2)</f>
+      <c r="Y3" s="1">
+        <f>SUM(Q8,Q7,Q6,S2)</f>
         <v>7.8191254034914424E+21</v>
       </c>
-      <c r="X3">
-        <f t="shared" ref="X3:X6" si="2">V3/B3</f>
+      <c r="Z3" s="1">
+        <f>X3/B3</f>
         <v>-1.4819130379366717E-3</v>
       </c>
-      <c r="Y3">
-        <f t="shared" ref="Y3:Y6" si="3">W3/B3</f>
+      <c r="AA3" s="1">
+        <f>Y3/B3</f>
         <v>1.2755506367849009E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -779,11 +811,11 @@
         <v>2.2899999999999998E+23</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ref="C4" si="4">E4*1.496 * 10 ^ 8</f>
+        <f t="shared" ref="C4" si="2">E4*1.496 * 10 ^ 8</f>
         <v>9080720000</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:D14" si="5">F4*1.496*10^8</f>
+        <f t="shared" ref="D4:D14" si="3">F4*1.496*10^8</f>
         <v>15334000000</v>
       </c>
       <c r="E4" s="1">
@@ -792,69 +824,72 @@
       <c r="F4" s="1">
         <v>102.5</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>1</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>4</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <f>SQRT((C2-C5)^2 + (D2-D5)^2)</f>
         <v>1094997647.0932896</v>
       </c>
-      <c r="J4">
-        <f>(C5-C2)/I4</f>
+      <c r="L4">
+        <f>(C5-C2)/K4</f>
         <v>0.32106005061584247</v>
       </c>
-      <c r="K4">
-        <f>(D5-D2)/I4</f>
+      <c r="M4">
+        <f>(D5-D2)/K4</f>
         <v>0.94705883866766827</v>
       </c>
-      <c r="L4" s="4">
-        <f t="shared" ref="L4:L21" si="6">-J4</f>
+      <c r="N4" s="4">
+        <f t="shared" ref="N4:N21" si="4">-L4</f>
         <v>-0.32106005061584247</v>
       </c>
-      <c r="M4" s="4">
-        <f t="shared" ref="M4:M21" si="7">-K4</f>
+      <c r="O4" s="4">
+        <f t="shared" ref="O4:O21" si="5">-M4</f>
         <v>-0.94705883866766827</v>
       </c>
-      <c r="N4">
-        <f xml:space="preserve"> -S$2 *(B2 *B5) / (I4)^2 *L4</f>
+      <c r="P4">
+        <f xml:space="preserve"> -U$2 *(B2 *B5) / (K4)^2 *N4</f>
         <v>8.0482886008764026E+20</v>
       </c>
-      <c r="O4">
-        <f xml:space="preserve"> -S$2 *(B2 *B5) / (I4)^2 *M4</f>
+      <c r="Q4">
+        <f xml:space="preserve"> -U$2 *(B2 *B5) / (K4)^2 *O4</f>
         <v>2.3740738970755421E+21</v>
       </c>
-      <c r="P4" s="4">
+      <c r="R4" s="4">
         <f t="shared" si="0"/>
         <v>-8.0482886008764026E+20</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="S4" s="4">
         <f t="shared" si="1"/>
         <v>-2.3740738970755421E+21</v>
       </c>
-      <c r="U4">
+      <c r="U4" t="s">
+        <v>25</v>
+      </c>
+      <c r="W4" s="1">
         <v>3</v>
       </c>
-      <c r="V4">
-        <f>SUM(N9,N10,P3,P6)</f>
+      <c r="X4" s="1">
+        <f>SUM(P9,P10,R3,R6)</f>
         <v>-6.7138465553336333E+17</v>
       </c>
-      <c r="W4">
-        <f>SUM(O9,O10,Q3,Q6)</f>
+      <c r="Y4" s="1">
+        <f>SUM(Q9,Q10,S3,S6)</f>
         <v>-1.2987414927331274E+18</v>
       </c>
-      <c r="X4">
-        <f t="shared" si="2"/>
+      <c r="Z4" s="1">
+        <f>X4/B4</f>
         <v>-2.9318107228531152E-6</v>
       </c>
-      <c r="Y4">
-        <f t="shared" si="3"/>
+      <c r="AA4" s="1">
+        <f>Y4/B4</f>
         <v>-5.6713602302756664E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -863,11 +898,11 @@
         <v>1.477E+25</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" ref="C5" si="8">E5*1.496*10^8</f>
+        <f t="shared" ref="C5" si="6">E5*1.496*10^8</f>
         <v>568480000</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>1900219200</v>
       </c>
       <c r="E5" s="1">
@@ -876,69 +911,72 @@
       <c r="F5" s="1">
         <v>12.702</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>1</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>5</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <f>SQRT((C2-C6)^2 + (D2-D6)^2)</f>
         <v>16499152795.913857</v>
       </c>
-      <c r="J5">
-        <f>(C6-C2)/I5</f>
+      <c r="L5">
+        <f>(C6-C2)/K5</f>
         <v>0.9351840176800652</v>
       </c>
-      <c r="K5">
-        <f>(D6-D2)/I5</f>
+      <c r="M5">
+        <f>(D6-D2)/K5</f>
         <v>0.35416218470606303</v>
       </c>
-      <c r="L5" s="4">
-        <f t="shared" si="6"/>
+      <c r="N5" s="4">
+        <f t="shared" si="4"/>
         <v>-0.9351840176800652</v>
       </c>
-      <c r="M5" s="4">
-        <f t="shared" si="7"/>
+      <c r="O5" s="4">
+        <f t="shared" si="5"/>
         <v>-0.35416218470606303</v>
       </c>
-      <c r="N5">
-        <f xml:space="preserve"> -S$2 *(B2 *B6) / (I5)^2 *L5</f>
+      <c r="P5">
+        <f xml:space="preserve"> -U$2 *(B2 *B6) / (K5)^2 *N5</f>
         <v>6.3019326934935603E+17</v>
       </c>
-      <c r="O5">
-        <f xml:space="preserve"> -S$2 *(B2 *B6) / (I5)^2 *M5</f>
+      <c r="Q5">
+        <f xml:space="preserve"> -U$2 *(B2 *B6) / (K5)^2 *O5</f>
         <v>2.3865958018989571E+17</v>
       </c>
-      <c r="P5" s="4">
-        <f xml:space="preserve"> -N5</f>
+      <c r="R5" s="4">
+        <f xml:space="preserve"> -P5</f>
         <v>-6.3019326934935603E+17</v>
       </c>
-      <c r="Q5" s="4">
-        <f xml:space="preserve"> -O5</f>
+      <c r="S5" s="4">
+        <f xml:space="preserve"> -Q5</f>
         <v>-2.3865958018989571E+17</v>
       </c>
       <c r="U5">
+        <v>500</v>
+      </c>
+      <c r="W5" s="1">
         <v>4</v>
       </c>
-      <c r="V5">
-        <f>SUM(N11,P4,P7,P9)</f>
+      <c r="X5" s="1">
+        <f>SUM(P11,R4,R7,R9)</f>
         <v>7.1946104103851168E+21</v>
       </c>
-      <c r="W5">
-        <f>SUM(O11,Q9,Q7,Q4)</f>
+      <c r="Y5" s="1">
+        <f>SUM(Q11,S9,S7,S4)</f>
         <v>-1.0852110566190496E+22</v>
       </c>
-      <c r="X5">
-        <f t="shared" si="2"/>
+      <c r="Z5" s="1">
+        <f>X5/B5</f>
         <v>4.8710970957245201E-4</v>
       </c>
-      <c r="Y5">
-        <f t="shared" si="3"/>
+      <c r="AA5" s="1">
+        <f>Y5/B5</f>
         <v>-7.3474005187477965E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -947,11 +985,11 @@
         <v>9.0143999999999992E+23</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" ref="C6" si="9">E6*1.496 * 10 ^ 8</f>
+        <f t="shared" ref="C6" si="7">E6*1.496 * 10 ^ 8</f>
         <v>15646664000.000002</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>6706568000</v>
       </c>
       <c r="E6" s="1">
@@ -960,531 +998,685 @@
       <c r="F6" s="1">
         <v>44.83</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>2</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>3</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <f>SQRT((C3-C4)^2 + (D3-D4)^2)</f>
         <v>16096873523.737976</v>
       </c>
-      <c r="J6">
-        <f>(C4-C3)/I6</f>
+      <c r="L6">
+        <f>(C4-C3)/K6</f>
         <v>0.49812535261431434</v>
       </c>
-      <c r="K6">
-        <f>(D4-D3)/I6</f>
+      <c r="M6">
+        <f>(D4-D3)/K6</f>
         <v>0.86710503001820083</v>
       </c>
-      <c r="L6" s="4">
-        <f t="shared" si="6"/>
+      <c r="N6" s="4">
+        <f t="shared" si="4"/>
         <v>-0.49812535261431434</v>
       </c>
-      <c r="M6" s="4">
-        <f t="shared" si="7"/>
+      <c r="O6" s="4">
+        <f t="shared" si="5"/>
         <v>-0.86710503001820083</v>
       </c>
-      <c r="N6">
-        <f xml:space="preserve"> -S$2 *(B3*B4) / I6^2 *L6</f>
+      <c r="P6">
+        <f xml:space="preserve"> -U$2 *(B3*B4) / K6^2 *N6</f>
         <v>1.8011806106550595E+17</v>
       </c>
-      <c r="O6">
-        <f xml:space="preserve"> -S$2 *(B3*B4) / I6^2 *M6</f>
+      <c r="Q6">
+        <f xml:space="preserve"> -U$2 *(B3*B4) / K6^2 *O6</f>
         <v>3.1353810025395923E+17</v>
       </c>
-      <c r="P6" s="4">
+      <c r="R6" s="4">
         <f t="shared" si="0"/>
         <v>-1.8011806106550595E+17</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="S6" s="4">
         <f t="shared" si="1"/>
         <v>-3.1353810025395923E+17</v>
       </c>
-      <c r="U6">
+      <c r="W6" s="1">
         <v>5</v>
       </c>
-      <c r="V6">
-        <f>SUM(P11,P10,P8,P5)</f>
+      <c r="X6" s="1">
+        <f>SUM(R11,R10,R8,R5)</f>
         <v>-5.5183853997845422E+18</v>
       </c>
-      <c r="W6">
-        <f>SUM(Q11,Q10,Q8,Q5)</f>
+      <c r="Y6" s="1">
+        <f>SUM(S11,S10,S8,S5)</f>
         <v>-1.7480479692639642E+18</v>
       </c>
-      <c r="X6">
-        <f t="shared" si="2"/>
+      <c r="Z6" s="1">
+        <f>X6/B6</f>
         <v>-6.1217445418270132E-6</v>
       </c>
-      <c r="Y6">
+      <c r="AA6" s="1">
+        <f>Y6/B6</f>
+        <v>-1.9391728448526405E-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="C7" s="1">
+        <f t="shared" ref="C7" si="8">E7*1.496*10^8</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
         <f t="shared" si="3"/>
-        <v>-1.9391728448526405E-6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="C7" s="1">
-        <f t="shared" ref="C7" si="10">E7*1.496*10^8</f>
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="I7">
         <v>2</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>4</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <f xml:space="preserve"> SQRT((C3-C5)^2 +(D3-D5)^2)</f>
         <v>720059596.00110877</v>
       </c>
-      <c r="J7">
-        <f>(C5-C3)/I7</f>
+      <c r="L7">
+        <f>(C5-C3)/K7</f>
         <v>-0.68602543837113084</v>
       </c>
-      <c r="K7">
-        <f>(D5-D3)/I7</f>
+      <c r="M7">
+        <f>(D5-D3)/K7</f>
         <v>0.72757755456562689</v>
       </c>
-      <c r="L7" s="4">
-        <f t="shared" si="6"/>
+      <c r="N7" s="4">
+        <f t="shared" si="4"/>
         <v>0.68602543837113084</v>
       </c>
-      <c r="M7" s="4">
-        <f t="shared" si="7"/>
+      <c r="O7" s="4">
+        <f t="shared" si="5"/>
         <v>-0.72757755456562689</v>
       </c>
-      <c r="N7">
-        <f xml:space="preserve"> -S$2 *(B3*B5) / I7^2 * L7</f>
+      <c r="P7">
+        <f xml:space="preserve"> -U$2 *(B3*B5) / K7^2 * N7</f>
         <v>-7.9955810231022172E+21</v>
       </c>
-      <c r="O7">
-        <f xml:space="preserve"> -S$2 *(B3*B5) /I7^2 *M7</f>
+      <c r="Q7">
+        <f xml:space="preserve"> -U$2 *(B3*B5) /K7^2 *O7</f>
         <v>8.4798681837988982E+21</v>
       </c>
-      <c r="P7" s="4">
+      <c r="R7" s="4">
         <f t="shared" si="0"/>
         <v>7.9955810231022172E+21</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="S7" s="4">
         <f t="shared" si="1"/>
         <v>-8.4798681837988982E+21</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C8" s="1">
-        <f t="shared" ref="C8" si="11">E8*1.496 * 10 ^ 8</f>
+        <f t="shared" ref="C8" si="9">E8*1.496 * 10 ^ 8</f>
         <v>0</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I8">
         <v>2</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>5</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <f xml:space="preserve"> SQRT((C3-C6)^2 +(D3-D6)^2)</f>
         <v>15527735616.948374</v>
       </c>
-      <c r="J8">
-        <f>(C6-C3)/I8</f>
+      <c r="L8">
+        <f>(C6-C3)/K8</f>
         <v>0.93923577524603674</v>
       </c>
-      <c r="K8">
-        <f>(D6-D3)/I8</f>
+      <c r="M8">
+        <f>(D6-D3)/K8</f>
         <v>0.3432727173807677</v>
       </c>
-      <c r="L8" s="4">
-        <f t="shared" si="6"/>
+      <c r="N8" s="4">
+        <f t="shared" si="4"/>
         <v>-0.93923577524603674</v>
       </c>
-      <c r="M8" s="4">
-        <f t="shared" si="7"/>
+      <c r="O8" s="4">
+        <f t="shared" si="5"/>
         <v>-0.3432727173807677</v>
       </c>
-      <c r="N8">
-        <f xml:space="preserve"> -S$2 *(B3*B6) / I8^2 *L8</f>
+      <c r="P8">
+        <f xml:space="preserve"> -U$2 *(B3*B6) / K8^2 *N8</f>
         <v>1.4366844593404408E+18</v>
       </c>
-      <c r="O8">
-        <f xml:space="preserve"> -S$2 *(B3*B6) /I8^2 *M8</f>
+      <c r="Q8">
+        <f xml:space="preserve"> -U$2 *(B3*B6) /K8^2 *O8</f>
         <v>5.2508070004820998E+17</v>
       </c>
-      <c r="P8" s="4">
+      <c r="R8" s="4">
         <f t="shared" si="0"/>
         <v>-1.4366844593404408E+18</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="S8" s="4">
         <f t="shared" si="1"/>
         <v>-5.2508070004820998E+17</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C9" s="1">
-        <f t="shared" ref="C9" si="12">E9*1.496*10^8</f>
+        <f t="shared" ref="C9" si="10">E9*1.496*10^8</f>
         <v>0</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I9">
         <v>3</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>4</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <f xml:space="preserve"> SQRT((C4-C5)^2 +(D4-D5)^2)</f>
         <v>15903606396.03636</v>
       </c>
-      <c r="J9">
-        <f>(C5-C4)/I9</f>
+      <c r="L9">
+        <f>(C5-C4)/K9</f>
         <v>-0.53523960465479692</v>
       </c>
-      <c r="K9">
-        <f>(D5-D4)/I9</f>
+      <c r="M9">
+        <f>(D5-D4)/K9</f>
         <v>-0.84470028152533305</v>
       </c>
-      <c r="L9" s="4">
-        <f t="shared" si="6"/>
+      <c r="N9" s="4">
+        <f t="shared" si="4"/>
         <v>0.53523960465479692</v>
       </c>
-      <c r="M9" s="4">
-        <f t="shared" si="7"/>
+      <c r="O9" s="4">
+        <f t="shared" si="5"/>
         <v>0.84470028152533305</v>
       </c>
-      <c r="N9">
-        <f xml:space="preserve"> -S$2 *(B4*B5) / I9^2 *L9</f>
+      <c r="P9">
+        <f xml:space="preserve"> -U$2 *(B4*B5) / K9^2 *N9</f>
         <v>-4.7772580970854381E+17</v>
       </c>
-      <c r="O9">
-        <f xml:space="preserve"> -S$2 *(B4*B5) / I9^2 *M9</f>
+      <c r="Q9">
+        <f xml:space="preserve"> -U$2 *(B4*B5) / K9^2 *O9</f>
         <v>-7.539336073850231E+17</v>
       </c>
-      <c r="P9" s="4">
+      <c r="R9" s="4">
         <f t="shared" si="0"/>
         <v>4.7772580970854381E+17</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="S9" s="4">
         <f t="shared" si="1"/>
         <v>7.539336073850231E+17</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="W9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="X9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="5"/>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C10" s="1">
-        <f t="shared" ref="C10" si="13">E10*1.496 * 10 ^ 8</f>
+        <f t="shared" ref="C10" si="11">E10*1.496 * 10 ^ 8</f>
         <v>0</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I10">
         <v>3</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>5</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <f xml:space="preserve"> SQRT((C4-C6)^2 +(D4-D6)^2)</f>
         <v>10841780459.212408</v>
       </c>
-      <c r="J10">
-        <f>(C6-C4)/I10</f>
+      <c r="L10">
+        <f>(C6-C4)/K10</f>
         <v>0.60561491949607138</v>
       </c>
-      <c r="K10">
-        <f>(D6-D4)/I10</f>
+      <c r="M10">
+        <f>(D6-D4)/K10</f>
         <v>-0.79575785844926916</v>
       </c>
-      <c r="L10" s="4">
-        <f t="shared" si="6"/>
+      <c r="N10" s="4">
+        <f t="shared" si="4"/>
         <v>-0.60561491949607138</v>
       </c>
-      <c r="M10" s="4">
-        <f t="shared" si="7"/>
+      <c r="O10" s="4">
+        <f t="shared" si="5"/>
         <v>0.79575785844926916</v>
       </c>
-      <c r="N10">
-        <f xml:space="preserve"> -S$2 *(B4*B6) / I10^2 *L10</f>
+      <c r="P10">
+        <f xml:space="preserve"> -U$2 *(B4*B6) / K10^2 *N10</f>
         <v>7.09861102626006E+16</v>
       </c>
-      <c r="O10">
-        <f xml:space="preserve"> -S$2 *(B4*B6) /I10^2 *M10</f>
+      <c r="Q10">
+        <f xml:space="preserve"> -U$2 *(B4*B6) /K10^2 *O10</f>
         <v>-9.3273387533474032E+16</v>
       </c>
-      <c r="P10" s="4">
+      <c r="R10" s="4">
         <f t="shared" si="0"/>
         <v>-7.09861102626006E+16</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="S10" s="4">
         <f t="shared" si="1"/>
         <v>9.3273387533474032E+16</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="W10" s="5">
+        <v>1</v>
+      </c>
+      <c r="X10" s="5">
+        <f>Z2 * U$5</f>
+        <v>0.3108734473961951</v>
+      </c>
+      <c r="Y10" s="5">
+        <f>AA2 *U$5</f>
+        <v>0.49787339327009705</v>
+      </c>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="5"/>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C11" s="1">
-        <f t="shared" ref="C11" si="14">E11*1.496*10^8</f>
+        <f t="shared" ref="C11" si="12">E11*1.496*10^8</f>
         <v>0</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I11">
         <v>4</v>
       </c>
-      <c r="H11">
+      <c r="J11">
         <v>5</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <f xml:space="preserve"> SQRT((C5-C6)^2 +(D5-D6)^2)</f>
         <v>15825694977.634237</v>
       </c>
-      <c r="J11">
-        <f>(C6-C5)/I11</f>
+      <c r="L11">
+        <f>(C6-C5)/K11</f>
         <v>0.95276599361414083</v>
       </c>
-      <c r="K11">
-        <f>(D6-D5)/I11</f>
+      <c r="M11">
+        <f>(D6-D5)/K11</f>
         <v>0.30370538587989993</v>
       </c>
-      <c r="L11" s="4">
-        <f t="shared" si="6"/>
+      <c r="N11" s="4">
+        <f t="shared" si="4"/>
         <v>-0.95276599361414083</v>
       </c>
-      <c r="M11" s="4">
-        <f t="shared" si="7"/>
+      <c r="O11" s="4">
+        <f t="shared" si="5"/>
         <v>-0.30370538587989993</v>
       </c>
-      <c r="N11">
-        <f xml:space="preserve"> -S$2 *(B5*B6) /I11^2 *L11</f>
+      <c r="P11">
+        <f xml:space="preserve"> -U$2 *(B5*B6) /K11^2 *N11</f>
         <v>3.3805215608321444E+18</v>
       </c>
-      <c r="O11">
-        <f xml:space="preserve"> -S$2 *(B5*B6) /I11^2 *M11</f>
+      <c r="Q11">
+        <f xml:space="preserve"> -U$2 *(B5*B6) /K11^2 *O11</f>
         <v>1.0775810765593325E+18</v>
       </c>
-      <c r="P11" s="4">
+      <c r="R11" s="4">
         <f t="shared" si="0"/>
         <v>-3.3805215608321444E+18</v>
       </c>
-      <c r="Q11" s="4">
+      <c r="S11" s="4">
         <f t="shared" si="1"/>
         <v>-1.0775810765593325E+18</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="W11" s="5">
+        <v>2</v>
+      </c>
+      <c r="X11" s="5">
+        <f t="shared" ref="X11:X13" si="13">Z3 * U$5</f>
+        <v>-0.74095651896833581</v>
+      </c>
+      <c r="Y11" s="5">
+        <f t="shared" ref="Y11:Y13" si="14">AA3 *U$5</f>
+        <v>0.6377753183924505</v>
+      </c>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="5"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C12" s="1">
         <f t="shared" ref="C12" si="15">E12*1.496 * 10 ^ 8</f>
         <v>0</v>
       </c>
       <c r="D12" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="L12" s="4">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M12" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P12" s="4">
+      <c r="R12" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q12" s="4">
+      <c r="S12" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="W12" s="5">
+        <v>3</v>
+      </c>
+      <c r="X12" s="5">
+        <f t="shared" si="13"/>
+        <v>-1.4659053614265577E-3</v>
+      </c>
+      <c r="Y12" s="5">
+        <f t="shared" si="14"/>
+        <v>-2.835680115137833E-3</v>
+      </c>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="5"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C13" s="1">
         <f t="shared" ref="C13" si="16">E13*1.496*10^8</f>
         <v>0</v>
       </c>
       <c r="D13" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="L13" s="4">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M13" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="4">
+      <c r="R13" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q13" s="4">
+      <c r="S13" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="W13" s="5">
+        <v>4</v>
+      </c>
+      <c r="X13" s="5">
+        <f t="shared" si="13"/>
+        <v>0.24355485478622602</v>
+      </c>
+      <c r="Y13" s="5">
+        <f t="shared" si="14"/>
+        <v>-0.36737002593738982</v>
+      </c>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="5"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C14" s="1">
         <f t="shared" ref="C14" si="17">E14*1.496 * 10 ^ 8</f>
         <v>0</v>
       </c>
       <c r="D14" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N14" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="L14" s="4">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M14" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P14" s="4">
+      <c r="R14" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q14" s="4">
+      <c r="S14" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="L15" s="4">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M15" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P15" s="4">
+      <c r="W14" s="5">
+        <v>5</v>
+      </c>
+      <c r="X14" s="5">
+        <f>Z6 * U$5</f>
+        <v>-3.0608722709135065E-3</v>
+      </c>
+      <c r="Y14" s="5">
+        <f>AA6 *U$5</f>
+        <v>-9.695864224263202E-4</v>
+      </c>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="5"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="N15" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O15" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R15" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q15" s="4">
+      <c r="S15" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="L16" s="4">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M16" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P16" s="4">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="N16" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R16" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q16" s="4">
+      <c r="S16" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="12:17" x14ac:dyDescent="0.3">
-      <c r="L17" s="4">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M17" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P17" s="4">
+    <row r="17" spans="14:27" x14ac:dyDescent="0.3">
+      <c r="N17" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R17" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q17" s="4">
+      <c r="S17" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="12:17" x14ac:dyDescent="0.3">
-      <c r="L18" s="4">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M18" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P18" s="4">
+      <c r="W17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="X17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z17" s="6"/>
+      <c r="AA17" s="6"/>
+    </row>
+    <row r="18" spans="14:27" x14ac:dyDescent="0.3">
+      <c r="N18" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R18" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q18" s="4">
+      <c r="S18" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="12:17" x14ac:dyDescent="0.3">
-      <c r="L19" s="4">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M19" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P19" s="4">
+      <c r="W18" s="6">
+        <v>1</v>
+      </c>
+      <c r="X18" s="6">
+        <f xml:space="preserve"> C2 + X10 *U$5</f>
+        <v>216920155.43672371</v>
+      </c>
+      <c r="Y18" s="6">
+        <f xml:space="preserve"> D2 +Y10 *U$5</f>
+        <v>863192248.93669653</v>
+      </c>
+      <c r="Z18" s="6"/>
+      <c r="AA18" s="6"/>
+    </row>
+    <row r="19" spans="14:27" x14ac:dyDescent="0.3">
+      <c r="N19" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R19" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q19" s="4">
+      <c r="S19" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="12:17" x14ac:dyDescent="0.3">
-      <c r="L20" s="4">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M20" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P20" s="4">
+      <c r="W19" s="6">
+        <v>2</v>
+      </c>
+      <c r="X19" s="6">
+        <f t="shared" ref="X19:X22" si="18" xml:space="preserve"> C3 + X11 *U$5</f>
+        <v>1062458829.5217406</v>
+      </c>
+      <c r="Y19" s="6">
+        <f t="shared" ref="Y19:Y22" si="19" xml:space="preserve"> D3 +Y11 *U$5</f>
+        <v>1376320318.8876593</v>
+      </c>
+      <c r="Z19" s="6"/>
+      <c r="AA19" s="6"/>
+    </row>
+    <row r="20" spans="14:27" x14ac:dyDescent="0.3">
+      <c r="N20" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R20" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q20" s="4">
+      <c r="S20" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="12:17" x14ac:dyDescent="0.3">
-      <c r="L21" s="4">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="M21" s="4">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P21" s="4">
+      <c r="W20" s="6">
+        <v>3</v>
+      </c>
+      <c r="X20" s="6">
+        <f t="shared" si="18"/>
+        <v>9080719999.2670479</v>
+      </c>
+      <c r="Y20" s="6">
+        <f t="shared" si="19"/>
+        <v>15333999998.582159</v>
+      </c>
+      <c r="Z20" s="6"/>
+      <c r="AA20" s="6"/>
+    </row>
+    <row r="21" spans="14:27" x14ac:dyDescent="0.3">
+      <c r="N21" s="4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O21" s="4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R21" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q21" s="4">
+      <c r="S21" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="W21" s="6">
+        <v>4</v>
+      </c>
+      <c r="X21" s="6">
+        <f t="shared" si="18"/>
+        <v>568480121.77742743</v>
+      </c>
+      <c r="Y21" s="6">
+        <f t="shared" si="19"/>
+        <v>1900219016.3149869</v>
+      </c>
+      <c r="Z21" s="6"/>
+      <c r="AA21" s="6"/>
+    </row>
+    <row r="22" spans="14:27" x14ac:dyDescent="0.3">
+      <c r="W22" s="6">
+        <v>5</v>
+      </c>
+      <c r="X22" s="6">
+        <f t="shared" si="18"/>
+        <v>15646663998.469566</v>
+      </c>
+      <c r="Y22" s="6">
+        <f t="shared" si="19"/>
+        <v>6706567999.5152063</v>
+      </c>
+      <c r="Z22" s="6"/>
+      <c r="AA22" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>